<commit_message>
SDTM Model and IG Updates
Bug fixes for loading all versions of SDTM Model and IG plus addition
of TTL and JSON exports for Model and IG
</commit_message>
<xml_diff>
--- a/public/upload/sdtm-3-1-3-excel.xlsx
+++ b/public/upload/sdtm-3-1-3-excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="27820" windowHeight="11420" tabRatio="860" activeTab="1"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="35840" windowHeight="17940" tabRatio="860"/>
   </bookViews>
   <sheets>
     <sheet name="SDTM 1.3 SDTMIG 3.1.3" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,12 @@
     <definedName name="Z_9CA9EE55_9E60_CF4D_8BDE_A47B53F67DC9_.wvu.FilterData" localSheetId="0" hidden="1">'SDTM 1.3 SDTMIG 3.1.3'!$B$1:$M$1</definedName>
     <definedName name="Z_9CA9EE55_9E60_CF4D_8BDE_A47B53F67DC9_.wvu.PrintArea" localSheetId="0" hidden="1">'SDTM 1.3 SDTMIG 3.1.3'!$A:$L</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anthony Chow - Personal View" guid="{82D46257-41BF-4117-B40B-1A01981D3099}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1688" yWindow="-8" windowWidth="1696" windowHeight="1036" tabRatio="860" activeSheetId="1"/>
+    <customWorkbookView name="Amy - Personal View" guid="{3D2B6433-1329-44FB-B7DE-D24CF7109B21}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1362" windowHeight="538" tabRatio="860" activeSheetId="1"/>
+    <customWorkbookView name="Wayne Kubick - Personal View" guid="{9CA9EE55-9E60-CF4D-8BDE-A47B53F67DC9}" mergeInterval="0" personalView="1" xWindow="407" yWindow="54" windowWidth="1037" windowHeight="722" tabRatio="860" activeSheetId="1"/>
     <customWorkbookView name="jchason - Personal View" guid="{856B09C9-8B94-4346-8227-95762479F1DB}" mergeInterval="0" personalView="1" xWindow="47" windowWidth="1871" windowHeight="1040" tabRatio="860" activeSheetId="1"/>
-    <customWorkbookView name="Wayne Kubick - Personal View" guid="{9CA9EE55-9E60-CF4D-8BDE-A47B53F67DC9}" mergeInterval="0" personalView="1" xWindow="407" yWindow="54" windowWidth="1037" windowHeight="722" tabRatio="860" activeSheetId="1"/>
-    <customWorkbookView name="Amy - Personal View" guid="{3D2B6433-1329-44FB-B7DE-D24CF7109B21}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1362" windowHeight="538" tabRatio="860" activeSheetId="1"/>
-    <customWorkbookView name="Anthony Chow - Personal View" guid="{82D46257-41BF-4117-B40B-1A01981D3099}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1688" yWindow="-8" windowWidth="1696" windowHeight="1036" tabRatio="860" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8851" uniqueCount="2383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8852" uniqueCount="2383">
   <si>
     <t>Contains the finding for all questions or sub-scores, copied or derived from QSORRES in a standard format or standard units. QSSTRESC should store all findings in character format; if findings are numeric, they should also be stored in numeric format in QSSTRESN. If question scores are derived from the original finding, then the standard format is the score. Examples: 0, 1. When sponsors apply codelist to indicate the code values are statistically meaningful standardized scores, which are defined by sponsors or by valid methodologies such as SF36 questionnaires, QSORRES will contain the decode format, and QSSTRESC and QSSTRESN may contain the standardized code values or scores.</t>
   </si>
@@ -7783,8 +7783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S969"/>
   <sheetViews>
-    <sheetView topLeftCell="B195" workbookViewId="0">
-      <selection activeCell="J195" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -34689,6 +34689,9 @@
       <c r="F846" s="4" t="s">
         <v>1868</v>
       </c>
+      <c r="G846" s="4" t="s">
+        <v>1114</v>
+      </c>
       <c r="H846" s="4" t="s">
         <v>1806</v>
       </c>
@@ -38678,25 +38681,9 @@
   <sheetProtection formatCells="0" formatColumns="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A1:L969"/>
   <customSheetViews>
-    <customSheetView guid="{856B09C9-8B94-4346-8227-95762479F1DB}" showPageBreaks="1" printArea="1" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A874" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A999" sqref="A999"/>
-      <printOptions horizontalCentered="1" gridLines="1"/>
-      <pageSetup scale="58" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-      <headerFooter>
-        <oddHeader>&amp;R&amp;"Arial,Bold"CDISC SDTM Implementation Guide (Version 3.1.3)</oddHeader>
-        <oddFooter>&amp;L&amp;8Page &amp;P_x000D_July 16, 2012&amp;R&amp;8© 2012 Clinical Data Interchange Standards Consortium, Inc. All rights reserved _x000D_Final_x000D_</oddFooter>
-      </headerFooter>
-      <autoFilter ref="B1:N1">
-        <filterColumn colId="0">
-          <customFilters and="1">
-            <customFilter operator="notEqual" val=" "/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{9CA9EE55-9E60-CF4D-8BDE-A47B53F67DC9}" scale="75" showAutoFilter="1" hiddenColumns="1">
-      <selection activeCell="F35" sqref="F35"/>
+    <customSheetView guid="{82D46257-41BF-4117-B40B-1A01981D3099}" printArea="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:N1048576"/>
       <printOptions horizontalCentered="1" gridLines="1"/>
       <pageSetup scale="58" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
       <headerFooter>
@@ -38715,9 +38702,8 @@
       </headerFooter>
       <autoFilter ref="B1:M1"/>
     </customSheetView>
-    <customSheetView guid="{82D46257-41BF-4117-B40B-1A01981D3099}" printArea="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:N1048576"/>
+    <customSheetView guid="{9CA9EE55-9E60-CF4D-8BDE-A47B53F67DC9}" scale="75" showAutoFilter="1" hiddenColumns="1">
+      <selection activeCell="F35" sqref="F35"/>
       <printOptions horizontalCentered="1" gridLines="1"/>
       <pageSetup scale="58" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
       <headerFooter>
@@ -38725,6 +38711,23 @@
         <oddFooter>&amp;L&amp;8Page &amp;P_x000D_July 16, 2012&amp;R&amp;8© 2012 Clinical Data Interchange Standards Consortium, Inc. All rights reserved _x000D_Final_x000D_</oddFooter>
       </headerFooter>
       <autoFilter ref="B1:M1"/>
+    </customSheetView>
+    <customSheetView guid="{856B09C9-8B94-4346-8227-95762479F1DB}" showPageBreaks="1" printArea="1" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A874" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A999" sqref="A999"/>
+      <printOptions horizontalCentered="1" gridLines="1"/>
+      <pageSetup scale="58" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+      <headerFooter>
+        <oddHeader>&amp;R&amp;"Arial,Bold"CDISC SDTM Implementation Guide (Version 3.1.3)</oddHeader>
+        <oddFooter>&amp;L&amp;8Page &amp;P_x000D_July 16, 2012&amp;R&amp;8© 2012 Clinical Data Interchange Standards Consortium, Inc. All rights reserved _x000D_Final_x000D_</oddFooter>
+      </headerFooter>
+      <autoFilter ref="B1:N1">
+        <filterColumn colId="0">
+          <customFilters and="1">
+            <customFilter operator="notEqual" val=" "/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -38747,7 +38750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -39456,7 +39459,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{856B09C9-8B94-4346-8227-95762479F1DB}">
+    <customSheetView guid="{82D46257-41BF-4117-B40B-1A01981D3099}">
+      <selection activeCell="D17" sqref="D17"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+    </customSheetView>
+    <customSheetView guid="{3D2B6433-1329-44FB-B7DE-D24CF7109B21}" showPageBreaks="1">
       <selection activeCell="D17" sqref="D17"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
     </customSheetView>
@@ -39464,11 +39471,7 @@
       <selection activeCell="D17" sqref="D17"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
     </customSheetView>
-    <customSheetView guid="{3D2B6433-1329-44FB-B7DE-D24CF7109B21}" showPageBreaks="1">
-      <selection activeCell="D17" sqref="D17"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
-    </customSheetView>
-    <customSheetView guid="{82D46257-41BF-4117-B40B-1A01981D3099}">
+    <customSheetView guid="{856B09C9-8B94-4346-8227-95762479F1DB}">
       <selection activeCell="D17" sqref="D17"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
     </customSheetView>

</xml_diff>